<commit_message>
DRAIAM101 new script has been developed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -295,6 +295,16 @@
   </si>
   <si>
     <t>Verify that STeAM account locked message sholud be displayed in an overlay as below " Your account has been locked for 30 minutes due to too many failed attempts." &lt;Okay&gt;||Verify that STeAM account is suspended message sholud be displayed in an overlay as below " Your account has been evicted. To get help, please email ProjectNeon@tr.com. &lt;Okay&gt;</t>
+  </si>
+  <si>
+    <t>DRAIAM101</t>
+  </si>
+  <si>
+    <t>OPQA-5162 || OPQA-5164</t>
+  </si>
+  <si>
+    <t>Verify that Thomson Reuters logo should be replaced with Clarivate Analytics logo
+|| Verify that Clarivate Analytics logo should be Placed below the marketing area (centered).</t>
   </si>
 </sst>
 </file>
@@ -358,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -381,12 +391,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -397,17 +420,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,7 +434,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -753,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +798,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -789,13 +809,13 @@
       <c r="A2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2"/>
@@ -810,7 +830,7 @@
       <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
@@ -825,7 +845,7 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="2"/>
@@ -840,157 +860,157 @@
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="5"/>
@@ -1002,175 +1022,193 @@
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="10"/>
+      <c r="D19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="D22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="10"/>
+      <c r="D23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="5"/>
+      <c r="D24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
+      <c r="D25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
+      <c r="D26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
+      <c r="D27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
New DRA Script for CustomerCare
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>TCID</t>
   </si>
@@ -305,6 +305,15 @@
   <si>
     <t>Verify that Thomson Reuters logo should be replaced with Clarivate Analytics logo
 || Verify that Clarivate Analytics logo should be Placed below the marketing area (centered).</t>
+  </si>
+  <si>
+    <t>DRAIAM070</t>
+  </si>
+  <si>
+    <t>OPQA-5154</t>
+  </si>
+  <si>
+    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported</t>
   </si>
 </sst>
 </file>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,6 +1219,21 @@
       </c>
       <c r="E28" s="8"/>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
New Script for DRA Customercare
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -314,6 +314,18 @@
   </si>
   <si>
     <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported</t>
+  </si>
+  <si>
+    <t>DRAIAM071</t>
+  </si>
+  <si>
+    <t>OPQA-5168 || OPQA-5227</t>
+  </si>
+  <si>
+    <t>Verify that the web form provided to user should be application specific with following required fields
+1.Name 2.Organization 3.Contact details (email, telephone) 4.Issue Category 5.Country
+6.Description of issue ( a free form text box where a user can describe why they are contacting support) ||
+Verify that the web form provided to user will be application specific with following required fields (Name, Organization, email, telephone, Issue Category, Country, Description of issue)</t>
   </si>
 </sst>
 </file>
@@ -782,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,6 +1246,21 @@
       </c>
       <c r="E29" s="8"/>
     </row>
+    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
Added IPAIAM customer care scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -310,12 +310,6 @@
     <t>DRAIAM070</t>
   </si>
   <si>
-    <t>OPQA-5154</t>
-  </si>
-  <si>
-    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported</t>
-  </si>
-  <si>
     <t>DRAIAM071</t>
   </si>
   <si>
@@ -326,6 +320,12 @@
 1.Name 2.Organization 3.Contact details (email, telephone) 4.Issue Category 5.Country
 6.Description of issue ( a free form text box where a user can describe why they are contacting support) ||
 Verify that the web form provided to user will be application specific with following required fields (Name, Organization, email, telephone, Issue Category, Country, Description of issue)</t>
+  </si>
+  <si>
+    <t>OPQA-5154||OPQA-5230</t>
+  </si>
+  <si>
+    <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.</t>
   </si>
 </sst>
 </file>
@@ -797,7 +797,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,15 +1231,15 @@
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>5</v>
@@ -1248,13 +1248,13 @@
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Developed new automation script(DRAIAM102)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>TCID</t>
   </si>
@@ -326,6 +326,16 @@
   </si>
   <si>
     <t>Verify that a "Call us" section is present in customer care contact page with customer care contact details (region, phone numbers, hours of operation, language supported||Ensure that the page has "Support Request" and "Call us" sections.</t>
+  </si>
+  <si>
+    <t>DRAIAM102</t>
+  </si>
+  <si>
+    <t>Verify that 'EndNote' should be moved within the white area and should be above 'Forgot Password' text and center aligned
+|| Verify that Clarivate Analytics logo should be Placed below the marketing area (centered).</t>
+  </si>
+  <si>
+    <t>OPQA-5136 || OPQA-5137</t>
   </si>
 </sst>
 </file>
@@ -794,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,6 +1271,21 @@
       </c>
       <c r="E30" s="8"/>
     </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
Added New Customer care scripts for DRAIAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
   <si>
     <t>TCID</t>
   </si>
@@ -336,6 +336,42 @@
   </si>
   <si>
     <t>OPQA-5136 || OPQA-5137</t>
+  </si>
+  <si>
+    <t>DRAIAMCC004</t>
+  </si>
+  <si>
+    <t>OPQA-5229||OPQA-5230</t>
+  </si>
+  <si>
+    <t>Verify that Page should change header title for different title||Ensure that the page has "Support Request" and "Call us" sections.</t>
+  </si>
+  <si>
+    <t>DRAIAMCC003</t>
+  </si>
+  <si>
+    <t>OPQA-5174</t>
+  </si>
+  <si>
+    <t>Verify that the user should be able to select the issue type/category of the issue as an option.</t>
+  </si>
+  <si>
+    <t>OPQA-5169||OPQA-5170</t>
+  </si>
+  <si>
+    <t>Verify that error messages/validation alerts "Please enter at least 2 characters for name" should be displayed when 'name' field is empty or 'name' field contains less than two characters.||Verify that error messages/validation alerts "Please enter at least 2 characters for Organization Name " should be displayed when 'Organization Name' field is empty or 'Organization Name' field contains less than two characters.</t>
+  </si>
+  <si>
+    <t>OPQA-5171||OPQA-5172</t>
+  </si>
+  <si>
+    <t>Verify that error messages/validation alerts " Incorrect email address format. Please try again." should be displayed when user enters incorrect email address.||Verify that error messages/validation alerts "Incorrect phone number format. Please try again.." should be displayed when user enters incorrect phone number.</t>
+  </si>
+  <si>
+    <t>DRAIAMCC001</t>
+  </si>
+  <si>
+    <t>DRAIAMCC002</t>
   </si>
 </sst>
 </file>
@@ -804,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1322,66 @@
       </c>
       <c r="E31" s="8"/>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
Developed new automation script(DRAIAM103)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>TCID</t>
   </si>
@@ -372,6 +372,16 @@
   </si>
   <si>
     <t>DRAIAMCC002</t>
+  </si>
+  <si>
+    <t>DRAIAM103</t>
+  </si>
+  <si>
+    <t>OPQA-5139 || OPQA-5140</t>
+  </si>
+  <si>
+    <t>Verify that 'Project Neon' should be moved within the white area and should be above 'Forgot Password' text and center aligned
+|| Verify that Clarivate Analytics logo should be below the Marketing area.</t>
   </si>
 </sst>
 </file>
@@ -840,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,15 +1332,15 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -1339,48 +1349,63 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added new script for OPQA-5228
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
   <si>
     <t>TCID</t>
   </si>
@@ -382,6 +382,24 @@
   <si>
     <t>Verify that 'Project Neon' should be moved within the white area and should be above 'Forgot Password' text and center aligned
 || Verify that Clarivate Analytics logo should be below the Marketing area.</t>
+  </si>
+  <si>
+    <t>DRAIAM072</t>
+  </si>
+  <si>
+    <t>DRAIAM073</t>
+  </si>
+  <si>
+    <t>OPQA-5155</t>
+  </si>
+  <si>
+    <t>OPQA-5228</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to manually select any particular country and see contact details associated with it as per IPA Customer Care Contact Details.doc and DRA Customer Care Contact Details.doc documents</t>
+  </si>
+  <si>
+    <t>Verify that the page shall be accessible in both an authenticated and a non-authenticated state</t>
   </si>
 </sst>
 </file>
@@ -606,7 +624,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -641,7 +659,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -850,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,93 +1337,123 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="D34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B36" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="D37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Edited testcase for draiam
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed forgot password scripts in IAM Modules
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="13296" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -171,21 +171,6 @@
     <t>Verify that the STeAM Step Up Auth Modal should be presented to the user without a pre-populated email address when user has a valid Neon session token and is navigating within the same browser window.</t>
   </si>
   <si>
-    <t>OPQA-1934||
-OPQA-1935&amp;OPQA-3687||
-OPQA-4230||OPQA-4229||
-OPQA-4231||OPQA-4232||
-OPQA-4636||OPQA-4261||
-OPQA-4244||OPQA-4264||
-OPQA-4265||OPQA-4237||
-OPQA-4239||OPQA-4240||
-OPQA-4246||OPQA-4248||
-OPQA-4252</t>
-  </si>
-  <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
-  </si>
-  <si>
     <t>OPQA-4531||OPQA-4533||OPQA-4547||OPQA-4550</t>
   </si>
   <si>
@@ -325,13 +310,20 @@
   <si>
     <t>Verify that 'Project Neon' should be moved within the white area and should be above 'Forgot Password' text and center aligned
 || Verify that Clarivate Analytics logo should be below the Marketing area.</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+  </si>
+  <si>
+    <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||
+OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,7 +541,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,10 +573,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -616,7 +607,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -792,23 +782,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,9 +815,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="57.6">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -840,9 +830,9 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -855,9 +845,9 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -870,9 +860,9 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
@@ -885,9 +875,9 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="57.6">
       <c r="A6" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>15</v>
@@ -900,9 +890,9 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="A7" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>7</v>
@@ -915,9 +905,9 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>40</v>
@@ -930,9 +920,9 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>38</v>
@@ -945,9 +935,9 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>16</v>
@@ -960,9 +950,9 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="57.6">
       <c r="A11" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -975,9 +965,9 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8">
       <c r="A12" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
@@ -990,9 +980,9 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -1005,9 +995,9 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
@@ -1020,9 +1010,9 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
@@ -1035,9 +1025,9 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>29</v>
@@ -1050,9 +1040,9 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -1065,9 +1055,9 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="43.2">
       <c r="A18" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>33</v>
@@ -1080,12 +1070,12 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.2">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>34</v>
@@ -1095,9 +1085,9 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>36</v>
@@ -1110,9 +1100,9 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="28.8">
       <c r="A21" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>42</v>
@@ -1125,135 +1115,135 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="57.6">
       <c r="A22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="43.2">
+      <c r="A23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" ht="172.8">
+      <c r="A24" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="B24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="C25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" ht="43.2">
+      <c r="A26" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="B26" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="8" t="s">
+      <c r="D27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" ht="30.75" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="D28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8">
+      <c r="A29" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="B29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="D29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="28.8">
+      <c r="A30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed Scripts in DRAIAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="13296" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -306,17 +306,17 @@
 || Verify that Clarivate Analytics logo should be below the Marketing area.</t>
   </si>
   <si>
-    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
-  </si>
-  <si>
-    <t>OPQA-1934||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||
+    <t>OPQA-4176||OPQA-4178||OPQA-4179||OPQA-4182||OPQA-4187||OPQA-4189||OPQA-5192||OPQA-5194||OPQA-5190</t>
+  </si>
+  <si>
+    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "||Verify that Learn more link is displayed and navigated to the correct page or not||Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify that 'DRA_support@thomsonreuters.com' is replaced with ' Drug Research Advisor Customer Care.'||Verify the Updated DRA Sign in page is based on the UX guidelines given in the URL : https://thomsonreuters.invisionapp.com/boards/X92S3LMDMZFCP/</t>
+  </si>
+  <si>
+    <t>OPQA-1934||OPQA-5162||OPQA-5163||OPQA-1935&amp;OPQA-3687||OPQA-4230||OPQA-4229||OPQA-4231||OPQA-4232||OPQA-4636||OPQA-5121||
 OPQA-1950||OPQA-1951||OPQA-1953||OPQA-1949||OPQA-4261&amp;&amp;OPQA-1948||OPQA-4244||OPQA-4264||OPQA-4265||OPQA-4237||OPQA-4239||OPQA-4240||OPQA-4246||OPQA-4248||OPQA-4252||OPQA-5399||OPQA-5400</t>
   </si>
   <si>
-    <t>OPQA-4176||OPQA-4178||OPQA-4179||OPQA-4182||OPQA-4187||OPQA-4189||OPQA-5192||OPQA-5194||OPQA-5190</t>
-  </si>
-  <si>
-    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "||Verify that Learn more link is displayed and navigated to the correct page or not||Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify that 'DRA_support@thomsonreuters.com' is replaced with ' Drug Research Advisor Customer Care.'||Verify the Updated DRA Sign in page is based on the UX guidelines given in the URL : https://thomsonreuters.invisionapp.com/boards/X92S3LMDMZFCP/</t>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters logo should be replaced with Clarivate Analytics logo as per updated UX guidelines(https://thomsonreuters.invisionapp.com/share/XAACS4Z53#/screens/217761229)||Verify that 'Drug Research Advisor: Target Druggability' should be moved within the white area (above and centered over the 'Forgot Password' text).||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'Drug Research Advisor : Target Druggability' should be moved within the white area||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
   </si>
 </sst>
 </file>
@@ -775,17 +775,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -805,22 +805,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105">
+    <row r="2" spans="1:5" ht="86.4">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="45">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -835,7 +835,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="45">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -850,7 +850,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="60">
+    <row r="6" spans="1:5" ht="57.6">
       <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
@@ -880,7 +880,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="45">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
@@ -895,7 +895,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -925,7 +925,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -940,7 +940,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="60">
+    <row r="11" spans="1:5" ht="57.6">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -955,7 +955,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -970,7 +970,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="45">
+    <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -985,7 +985,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="43.2">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="45">
+    <row r="19" spans="1:5" ht="43.2">
       <c r="A19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="30">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>69</v>
       </c>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="28.8">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="60">
+    <row r="22" spans="1:5" ht="57.6">
       <c r="A22" s="7" t="s">
         <v>71</v>
       </c>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="45">
+    <row r="23" spans="1:5" ht="43.2">
       <c r="A23" s="7" t="s">
         <v>72</v>
       </c>
@@ -1135,15 +1135,15 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="180">
+    <row r="24" spans="1:5" ht="187.2">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>5</v>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="45">
+    <row r="26" spans="1:5" ht="43.2">
       <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="30">
+    <row r="29" spans="1:5" ht="28.8">
       <c r="A29" s="7" t="s">
         <v>82</v>
       </c>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Created DRASSOPage class and changed login, config perperties file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>TCID</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that Thomson Reuters logo should be replaced with Clarivate Analytics logo as per updated UX guidelines(https://thomsonreuters.invisionapp.com/share/XAACS4Z53#/screens/217761229)||Verify that 'Drug Research Advisor: Target Druggability' should be moved within the white area (above and centered over the 'Forgot Password' text).||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'Drug Research Advisor : Target Druggability' should be moved within the white area||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify  Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp;Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
+  </si>
+  <si>
+    <t>DRAIAM111</t>
+  </si>
+  <si>
+    <t>OP11</t>
+  </si>
+  <si>
+    <t>LogIn</t>
   </si>
 </sst>
 </file>
@@ -773,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1240,6 +1249,21 @@
       </c>
       <c r="E30" s="7"/>
     </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>

</xml_diff>

<commit_message>
Added DRA SSO testscripts for the Subflow 3 and 4.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13296" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>TCID</t>
   </si>
@@ -327,12 +328,18 @@
   <si>
     <t>LogIn</t>
   </si>
+  <si>
+    <t>DRAIAMSSO003</t>
+  </si>
+  <si>
+    <t>DRAIAMSSO004</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -417,11 +424,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -452,6 +472,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,9 +597,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,6 +632,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -781,23 +808,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -829,7 +856,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -844,7 +871,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -859,7 +886,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -874,7 +901,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="57.6">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
@@ -889,7 +916,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
@@ -904,7 +931,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -919,7 +946,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>58</v>
       </c>
@@ -934,7 +961,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="43.2">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -949,7 +976,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="57.6">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -964,7 +991,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -979,7 +1006,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="43.2">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -994,7 +1021,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1009,7 +1036,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1024,7 +1051,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1039,7 +1066,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1054,7 +1081,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="43.2">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1069,7 +1096,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="43.2">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1084,7 +1111,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>69</v>
       </c>
@@ -1099,7 +1126,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1114,7 +1141,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="57.6">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>71</v>
       </c>
@@ -1129,7 +1156,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="43.2">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>72</v>
       </c>
@@ -1144,7 +1171,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="187.2">
+    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1159,7 +1186,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>74</v>
       </c>
@@ -1174,7 +1201,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="43.2">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
@@ -1189,7 +1216,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -1204,7 +1231,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
@@ -1219,7 +1246,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="28.8">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>82</v>
       </c>
@@ -1234,7 +1261,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="28.8">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>
@@ -1249,7 +1276,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>92</v>
       </c>
@@ -1263,6 +1290,29 @@
         <v>5</v>
       </c>
       <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added new scripts in DRAIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
   <si>
     <t>TCID</t>
   </si>
@@ -326,6 +326,24 @@
   </si>
   <si>
     <t>LogIn</t>
+  </si>
+  <si>
+    <t>DRAIAM112</t>
+  </si>
+  <si>
+    <t>OP12</t>
+  </si>
+  <si>
+    <t>Suspend User</t>
+  </si>
+  <si>
+    <t>DRAIAM113</t>
+  </si>
+  <si>
+    <t>OP13</t>
+  </si>
+  <si>
+    <t>Evicted User</t>
   </si>
 </sst>
 </file>
@@ -782,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1264,6 +1282,36 @@
       </c>
       <c r="E31" s="7"/>
     </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>

</xml_diff>

<commit_message>
Added new script in DRAIAM Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>Existing User</t>
+  </si>
+  <si>
+    <t>DRAIAM114</t>
+  </si>
+  <si>
+    <t>OP114</t>
+  </si>
+  <si>
+    <t>New User</t>
   </si>
 </sst>
 </file>
@@ -815,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1329,11 +1338,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="C34" s="8" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -1342,7 +1353,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
@@ -1355,11 +1366,11 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B36" s="7"/>
-      <c r="C36" s="7" t="s">
-        <v>97</v>
+      <c r="C36" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1368,16 +1379,29 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="7"/>
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added test cases in excle sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
   <si>
     <t>TCID</t>
   </si>
@@ -322,9 +322,6 @@
     <t>DRAIAM111</t>
   </si>
   <si>
-    <t>OP11</t>
-  </si>
-  <si>
     <t>LogIn</t>
   </si>
   <si>
@@ -349,25 +346,34 @@
     <t>DRAIAM112</t>
   </si>
   <si>
-    <t>Suspend User</t>
-  </si>
-  <si>
     <t>DRAIAM113</t>
   </si>
   <si>
-    <t>OP113</t>
-  </si>
-  <si>
-    <t>Existing User</t>
-  </si>
-  <si>
     <t>DRAIAM114</t>
   </si>
   <si>
-    <t>OP114</t>
-  </si>
-  <si>
-    <t>New User</t>
+    <t>OPQA-5682</t>
+  </si>
+  <si>
+    <t>Verify the SSO authentication via WAYFLess/direct URL</t>
+  </si>
+  <si>
+    <t>OPQA-5689</t>
+  </si>
+  <si>
+    <t>verify that "Your account has been suspended Questions? Contact [Application_customer_care]" error message when user is an existing STeAM User that is suspended.</t>
+  </si>
+  <si>
+    <t>OPQA-5686</t>
+  </si>
+  <si>
+    <t>Verify that user able to login DRA ,If user doesn't exist in STeAM but exist in IdP.</t>
+  </si>
+  <si>
+    <t>Verify that user able to login DRA ,If user exist in STeAM but not associated any DRA SSO claimticket</t>
+  </si>
+  <si>
+    <t>OPQA-5694</t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1296,10 +1302,10 @@
         <v>92</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
@@ -1308,13 +1314,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -1323,13 +1329,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
@@ -1338,7 +1344,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>107</v>
@@ -1353,11 +1359,11 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1366,11 +1372,11 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1379,11 +1385,11 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -1392,11 +1398,11 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Created new SSO scripts in DRAIAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="120">
   <si>
     <t>TCID</t>
   </si>
@@ -374,6 +374,33 @@
   </si>
   <si>
     <t>OPQA-5694</t>
+  </si>
+  <si>
+    <t>DRAIAM115</t>
+  </si>
+  <si>
+    <t>OPQA-5683</t>
+  </si>
+  <si>
+    <t>Verify that user with both a TD and DD subscription shall be taken to the interoperability page after successful authentication</t>
+  </si>
+  <si>
+    <t>DRAIAM116</t>
+  </si>
+  <si>
+    <t>DRAIAM117</t>
+  </si>
+  <si>
+    <t>OPQA-5684</t>
+  </si>
+  <si>
+    <t>Verify that user with a TD-only subscription shall be taken to the TD homepage after successful authentication</t>
+  </si>
+  <si>
+    <t>OPQA-5685</t>
+  </si>
+  <si>
+    <t>Verify that user with a DD-only subscription shall be taken to the DD homepage after successful authentication</t>
   </si>
 </sst>
 </file>
@@ -830,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1359,11 +1386,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="7"/>
+        <v>111</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="C35" s="8" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1372,11 +1401,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="7"/>
+        <v>114</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="C36" s="8" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1385,11 +1416,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7" t="s">
-        <v>96</v>
+        <v>115</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -1398,16 +1431,55 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="7"/>
+      <c r="D41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated DRAIAM test cases and Replaced thread.sleep with fluent wait.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="5028"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17850" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
   <si>
     <t>TCID</t>
   </si>
@@ -322,6 +322,9 @@
     <t>DRAIAM111</t>
   </si>
   <si>
+    <t>OP11</t>
+  </si>
+  <si>
     <t>LogIn</t>
   </si>
   <si>
@@ -331,83 +334,36 @@
     <t>DRAIAMSSO004</t>
   </si>
   <si>
-    <t>SAML Response is invalid</t>
-  </si>
-  <si>
     <t>DRAIAMSSO008</t>
   </si>
   <si>
     <t>DRAIAMSSO009</t>
   </si>
   <si>
-    <t>Email is not released in saml attributes in saml response.</t>
-  </si>
-  <si>
-    <t>DRAIAM112</t>
-  </si>
-  <si>
-    <t>DRAIAM113</t>
-  </si>
-  <si>
-    <t>DRAIAM114</t>
-  </si>
-  <si>
-    <t>OPQA-5682</t>
-  </si>
-  <si>
-    <t>Verify the SSO authentication via WAYFLess/direct URL</t>
-  </si>
-  <si>
-    <t>OPQA-5689</t>
-  </si>
-  <si>
-    <t>verify that "Your account has been suspended Questions? Contact [Application_customer_care]" error message when user is an existing STeAM User that is suspended.</t>
-  </si>
-  <si>
-    <t>OPQA-5686</t>
-  </si>
-  <si>
-    <t>Verify that user able to login DRA ,If user doesn't exist in STeAM but exist in IdP.</t>
-  </si>
-  <si>
-    <t>Verify that user able to login DRA ,If user exist in STeAM but not associated any DRA SSO claimticket</t>
-  </si>
-  <si>
-    <t>OPQA-5694</t>
-  </si>
-  <si>
-    <t>DRAIAM115</t>
-  </si>
-  <si>
-    <t>OPQA-5683</t>
-  </si>
-  <si>
-    <t>Verify that user with both a TD and DD subscription shall be taken to the interoperability page after successful authentication</t>
-  </si>
-  <si>
-    <t>DRAIAM116</t>
-  </si>
-  <si>
-    <t>DRAIAM117</t>
-  </si>
-  <si>
-    <t>OPQA-5684</t>
-  </si>
-  <si>
-    <t>Verify that user with a TD-only subscription shall be taken to the TD homepage after successful authentication</t>
-  </si>
-  <si>
-    <t>OPQA-5685</t>
-  </si>
-  <si>
-    <t>Verify that user with a DD-only subscription shall be taken to the DD homepage after successful authentication</t>
+    <t>DRAIAMSSO006</t>
+  </si>
+  <si>
+    <t>Verify Error message when User is associated with one or more active UNP subscription(s) across other Neon Sub Apps.</t>
+  </si>
+  <si>
+    <t>Verify that "Thank you for your interest in Clarivate Analytics [Application_Name] is a subscription product.</t>
+  </si>
+  <si>
+    <t>Verify that "Access issue We are having an issue signing you into [Application_Name]. Refer to [AuthReqId].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Questions? Contact [Application_customer_care]." when User is already associated with a subscription for a given customer for a given app (UnP, tries SSO)</t>
+  </si>
+  <si>
+    <t>Verify that "The page you are looking for cannot be found.Questions? Contact [Application_customer_care]." error message when Email is not released in saml attributes in saml response.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -527,6 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +572,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -647,9 +604,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,6 +639,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -856,23 +815,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -904,7 +863,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -919,7 +878,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -934,7 +893,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -949,7 +908,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="57.6">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
@@ -964,7 +923,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
@@ -979,7 +938,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -994,7 +953,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>58</v>
       </c>
@@ -1009,7 +968,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="43.2">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -1024,7 +983,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="57.6">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1039,7 +998,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1054,7 +1013,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="43.2">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1069,7 +1028,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1084,7 +1043,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1099,7 +1058,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1114,7 +1073,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1129,7 +1088,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="43.2">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1144,7 +1103,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="43.2">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1159,7 +1118,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>69</v>
       </c>
@@ -1174,7 +1133,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1189,7 +1148,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="57.6">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>71</v>
       </c>
@@ -1204,7 +1163,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="43.2">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>72</v>
       </c>
@@ -1219,7 +1178,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="187.2">
+    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1234,7 +1193,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>74</v>
       </c>
@@ -1249,7 +1208,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="43.2">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
@@ -1264,7 +1223,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -1279,7 +1238,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
@@ -1294,7 +1253,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="28.8">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>82</v>
       </c>
@@ -1309,7 +1268,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="28.8">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>
@@ -1324,162 +1283,97 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="7" t="s">
-        <v>97</v>
-      </c>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
-      <c r="C40" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="7" t="s">
-        <v>98</v>
-      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
-      <c r="C41" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added new scripts in DRAIAM excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17850" windowHeight="5025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="5028"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
   <si>
     <t>TCID</t>
   </si>
@@ -322,12 +322,6 @@
     <t>DRAIAM111</t>
   </si>
   <si>
-    <t>OP11</t>
-  </si>
-  <si>
-    <t>LogIn</t>
-  </si>
-  <si>
     <t>DRAIAMSSO003</t>
   </si>
   <si>
@@ -357,13 +351,73 @@
   </si>
   <si>
     <t>Verify that "The page you are looking for cannot be found.Questions? Contact [Application_customer_care]." error message when Email is not released in saml attributes in saml response.</t>
+  </si>
+  <si>
+    <t>OPQA-5682</t>
+  </si>
+  <si>
+    <t>Verify the SSO authentication via WAYFLess/direct URL</t>
+  </si>
+  <si>
+    <t>DRAIAM112</t>
+  </si>
+  <si>
+    <t>OPQA-5689</t>
+  </si>
+  <si>
+    <t>verify that "Your account has been suspended Questions? Contact [Application_customer_care]" error message when user is an existing STeAM User that is suspended.</t>
+  </si>
+  <si>
+    <t>DRAIAM113</t>
+  </si>
+  <si>
+    <t>OPQA-5694</t>
+  </si>
+  <si>
+    <t>Verify that user able to login DRA ,If user exist in STeAM but not associated any DRA SSO claimticket</t>
+  </si>
+  <si>
+    <t>DRAIAM114</t>
+  </si>
+  <si>
+    <t>OPQA-5686</t>
+  </si>
+  <si>
+    <t>Verify that user able to login DRA ,If user doesn't exist in STeAM but exist in IdP.</t>
+  </si>
+  <si>
+    <t>DRAIAM115</t>
+  </si>
+  <si>
+    <t>OPQA-5683</t>
+  </si>
+  <si>
+    <t>Verify that user with both a TD and DD subscription shall be taken to the interoperability page after successful authentication</t>
+  </si>
+  <si>
+    <t>DRAIAM116</t>
+  </si>
+  <si>
+    <t>OPQA-5684</t>
+  </si>
+  <si>
+    <t>Verify that user with a TD-only subscription shall be taken to the TD homepage after successful authentication</t>
+  </si>
+  <si>
+    <t>DRAIAM117</t>
+  </si>
+  <si>
+    <t>OPQA-5685</t>
+  </si>
+  <si>
+    <t>Verify that user with a DD-only subscription shall be taken to the DD homepage after successful authentication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,7 +626,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,10 +658,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,7 +692,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -815,23 +867,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="86.4">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -863,7 +915,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -878,7 +930,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -893,7 +945,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -908,7 +960,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="57.6">
       <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
@@ -923,7 +975,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
@@ -938,7 +990,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -953,7 +1005,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>58</v>
       </c>
@@ -968,7 +1020,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -983,7 +1035,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="57.6">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -998,7 +1050,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1013,7 +1065,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="43.2">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1028,7 +1080,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1043,7 +1095,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1058,7 +1110,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1073,7 +1125,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1088,7 +1140,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="43.2">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1103,7 +1155,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.2">
       <c r="A19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1118,7 +1170,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>69</v>
       </c>
@@ -1133,7 +1185,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="28.8">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1148,7 +1200,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="57.6">
       <c r="A22" s="7" t="s">
         <v>71</v>
       </c>
@@ -1163,7 +1215,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="43.2">
       <c r="A23" s="7" t="s">
         <v>72</v>
       </c>
@@ -1178,7 +1230,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="187.2">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1193,7 +1245,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
         <v>74</v>
       </c>
@@ -1208,7 +1260,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="43.2">
       <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
@@ -1223,7 +1275,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -1238,7 +1290,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
@@ -1253,7 +1305,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8">
       <c r="A29" s="7" t="s">
         <v>82</v>
       </c>
@@ -1268,7 +1320,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>
@@ -1283,97 +1335,175 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" ht="28.8">
+      <c r="A42" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated DRA SSO Test cases in excel sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRAIAM.xlsx
+++ b/src/test/resources/xls/DRAIAM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="5028"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="128">
   <si>
     <t>TCID</t>
   </si>
@@ -346,10 +346,6 @@
     <t>Verify that "Access issue We are having an issue signing you into [Application_Name]. Refer to [AuthReqId].</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Questions? Contact [Application_customer_care]." when User is already associated with a subscription for a given customer for a given app (UnP, tries SSO)</t>
-  </si>
-  <si>
     <t>Verify that "The page you are looking for cannot be found.Questions? Contact [Application_customer_care]." error message when Email is not released in saml attributes in saml response.</t>
   </si>
   <si>
@@ -411,13 +407,31 @@
   </si>
   <si>
     <t>Verify that user with a DD-only subscription shall be taken to the DD homepage after successful authentication</t>
+  </si>
+  <si>
+    <t>OPQA-5687</t>
+  </si>
+  <si>
+    <t>OPQA-5688</t>
+  </si>
+  <si>
+    <t>OPQA-5690</t>
+  </si>
+  <si>
+    <t>Verify that  "Please sign in to [Application_Name] with the email address and password used to create your Clarivate Analytics account.</t>
+  </si>
+  <si>
+    <t>OPQA-5691</t>
+  </si>
+  <si>
+    <t>OPQA-5692</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,7 +640,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,9 +672,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -692,6 +707,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -867,23 +883,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="139.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="139.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -915,7 +931,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
@@ -930,7 +946,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="43.2">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -945,7 +961,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>54</v>
       </c>
@@ -960,7 +976,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="57.6">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
@@ -975,7 +991,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>56</v>
       </c>
@@ -990,7 +1006,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -1005,7 +1021,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>58</v>
       </c>
@@ -1020,7 +1036,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="43.2">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>59</v>
       </c>
@@ -1035,7 +1051,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="57.6">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1050,7 +1066,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1065,7 +1081,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="43.2">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1080,7 +1096,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1095,7 +1111,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1110,7 +1126,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
@@ -1125,7 +1141,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
@@ -1140,7 +1156,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="43.2">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>67</v>
       </c>
@@ -1155,7 +1171,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="43.2">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>68</v>
       </c>
@@ -1170,7 +1186,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>69</v>
       </c>
@@ -1185,7 +1201,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1200,7 +1216,7 @@
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="57.6">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>71</v>
       </c>
@@ -1215,7 +1231,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="43.2">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>72</v>
       </c>
@@ -1230,7 +1246,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="187.2">
+    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1245,7 +1261,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>74</v>
       </c>
@@ -1260,7 +1276,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" ht="43.2">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>75</v>
       </c>
@@ -1275,7 +1291,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -1290,7 +1306,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" ht="30.75" customHeight="1">
+    <row r="28" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
@@ -1305,7 +1321,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" ht="28.8">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>82</v>
       </c>
@@ -1320,7 +1336,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="28.8">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>85</v>
       </c>
@@ -1335,116 +1351,118 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="C38" s="8" t="s">
         <v>98</v>
       </c>
@@ -1453,11 +1471,13 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="7"/>
+      <c r="B39" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="C39" s="8" t="s">
         <v>99</v>
       </c>
@@ -1466,11 +1486,13 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="7"/>
+      <c r="B40" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="C40" s="8" t="s">
         <v>100</v>
       </c>
@@ -1479,26 +1501,30 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="7"/>
+      <c r="B41" s="7" t="s">
+        <v>126</v>
+      </c>
       <c r="C41" s="16" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" ht="28.8">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C42" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>5</v>
@@ -1512,8 +1538,13 @@
     <hyperlink ref="B13" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4223"/>
     <hyperlink ref="B15" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
     <hyperlink ref="B16:B17" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B38" r:id="rId6" display="https://jira.clarivate.io/browse/OPQA-5687"/>
+    <hyperlink ref="B39" r:id="rId7" display="https://jira.clarivate.io/browse/OPQA-5687"/>
+    <hyperlink ref="B40" r:id="rId8" display="https://jira.clarivate.io/browse/OPQA-5687"/>
+    <hyperlink ref="B41" r:id="rId9" display="https://jira.clarivate.io/browse/OPQA-5687"/>
+    <hyperlink ref="B42" r:id="rId10" display="https://jira.clarivate.io/browse/OPQA-5687"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>